<commit_message>
excel update for 2. milestone
</commit_message>
<xml_diff>
--- a/math_solve.xlsx
+++ b/math_solve.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AD5E84-E77B-4350-8DCE-0ACD834C4E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C212BEB3-FAEA-4F4A-847F-78ADF3C797AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D6196F6-7BF2-4472-84F1-499F220C9EB8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
   <si>
     <t>Feladat száma</t>
   </si>
@@ -324,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -347,7 +347,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -699,7 +698,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:F23"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,14 +898,14 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -922,7 +921,7 @@
       <c r="E13" s="1">
         <v>6</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -938,7 +937,7 @@
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="10"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -954,7 +953,7 @@
       <c r="E15" s="1">
         <v>7</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -986,7 +985,7 @@
       <c r="E17" s="1">
         <v>5</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -998,11 +997,13 @@
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E18" s="1">
         <v>5</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1011,14 +1012,14 @@
       <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1034,7 +1035,7 @@
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="10"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1052,7 +1053,7 @@
       <c r="E21" s="1">
         <v>4</v>
       </c>
-      <c r="F21" s="10"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1061,24 +1062,24 @@
       <c r="B22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
excel update for start the 3. milestone
</commit_message>
<xml_diff>
--- a/math_solve.xlsx
+++ b/math_solve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C212BEB3-FAEA-4F4A-847F-78ADF3C797AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEC3F28-CE5D-4FCE-99EA-E2A4F1BC6139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D6196F6-7BF2-4472-84F1-499F220C9EB8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>Feladat száma</t>
   </si>
@@ -195,13 +195,16 @@
   </si>
   <si>
     <t>Színek beállítása main pagen</t>
+  </si>
+  <si>
+    <t>Második ciklus vége (2025.02.28)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,8 +249,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +305,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -324,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -358,6 +374,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -695,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24176174-65B8-4DE0-80DA-06632CB27EA9}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="112" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,10 +1107,121 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="15"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="15"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="15"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A34:F34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update excel for milestone 3
</commit_message>
<xml_diff>
--- a/math_solve.xlsx
+++ b/math_solve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEC3F28-CE5D-4FCE-99EA-E2A4F1BC6139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32DEF01-8732-4FFA-9125-2CA70133F2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D6196F6-7BF2-4472-84F1-499F220C9EB8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="76">
   <si>
     <t>Feladat száma</t>
   </si>
@@ -197,7 +197,73 @@
     <t>Színek beállítása main pagen</t>
   </si>
   <si>
-    <t>Második ciklus vége (2025.02.28)</t>
+    <t>Hamradik ciklus vége (2025.02.28)</t>
+  </si>
+  <si>
+    <t>Main page szűrések kivitelezése</t>
+  </si>
+  <si>
+    <t>Heti/Havi kihívások design</t>
+  </si>
+  <si>
+    <t>Profil statisztika kivitelezésének megkezdése</t>
+  </si>
+  <si>
+    <t>Telós nézetek az oldalakhoz elkezdése</t>
+  </si>
+  <si>
+    <t>Közösségi oldal befejezése</t>
+  </si>
+  <si>
+    <t>Card designok befejezése</t>
+  </si>
+  <si>
+    <t>Admin panel elkészítése</t>
+  </si>
+  <si>
+    <t>Verseny feladatok kiosztásának a logikája</t>
+  </si>
+  <si>
+    <t>Verseny oldalak komponensek létrehozása</t>
+  </si>
+  <si>
+    <t>Clean code</t>
+  </si>
+  <si>
+    <t>Badge-ek megtervezése</t>
+  </si>
+  <si>
+    <t>Formapp-ba behúzás</t>
+  </si>
+  <si>
+    <t>Store page elkezése</t>
+  </si>
+  <si>
+    <t>Store-ok átszervezése</t>
+  </si>
+  <si>
+    <t>Lehúzások összesítése</t>
+  </si>
+  <si>
+    <t>VIP paraméterek kivitelezése</t>
+  </si>
+  <si>
+    <t>Feladatokhoz anyaggyűtés</t>
+  </si>
+  <si>
+    <t>Felhasználó feladat beküldésének lehetősége</t>
+  </si>
+  <si>
+    <t>Strake nézése napi feladatnál</t>
+  </si>
+  <si>
+    <t>Adatbázis átnézés/változtatása</t>
+  </si>
+  <si>
+    <t>40+1</t>
+  </si>
+  <si>
+    <t>emailok megtervezése</t>
   </si>
 </sst>
 </file>
@@ -250,14 +316,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,8 +378,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -335,10 +407,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -367,6 +455,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,18 +471,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -721,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24176174-65B8-4DE0-80DA-06632CB27EA9}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="112" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="112" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,14 +1013,14 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1098,130 +1187,326 @@
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="10"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="15"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="10"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="10"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+      <c r="B27" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="10"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="10"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="15"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="10"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="15"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="10"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="10"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>29</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="10"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="15"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>30</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
+      <c r="B33" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="10"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="15"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>31</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>32</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>33</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>34</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>35</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>38</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>39</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>40</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A45:F45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>